<commit_message>
Implemented atom-map-free reaction-center-mcs analysis and tested it on akg -> hopa expansion
</commit_message>
<xml_diff>
--- a/artifacts/pwy_xls/alpha_ketoglutarate_to_hopa_gen_2_tan_sample_0_n_samples_1000.xlsx
+++ b/artifacts/pwy_xls/alpha_ketoglutarate_to_hopa_gen_2_tan_sample_0_n_samples_1000.xlsx
@@ -482,7 +482,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -498,28 +498,28 @@
         <v>20.16037334979901</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.8882575757575757</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0.9583333333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8333333333333333</v>
+        <v>0.8181818181818181</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Q97UA1, P42236, Q08IC0, Q1JUP4, D4GP41, Q08IB7, Q6FFQ0</t>
+          <t>Q08IB7, P42236, Q1JUP4, Q08IC0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>O60218</t>
+          <t>Q3ZCJ2, Q9JII6, Q5R5D5, P50578, P14550, P51635, O70473</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -535,22 +535,22 @@
         <v>43.9738848645424</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.7626262626262625</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.7626262626262625</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Q5LVV1, Q46N53</t>
+          <t>Q8PLG9, O13471, Q8GKZ1, P62459, Q8X8T3, Q5LL27, Q47AL5, Q5FS83, O30027, P63952, P60859, Q5H0L1, Q492K3, Q5LAZ8, Q7MLS6, Q9L6I1, Q8PZR8, Q9F854, Q8XV79, Q3IQR5, P57201, Q7U8K7, Q7V004, Q318Q4, Q323J2, Q3A133, P62460, Q3MEV7, Q7M8K9, Q5F7D8, P60862, Q7NL02, Q722Y3, Q8DTQ7, Q67KH6, Q9C5U8, Q64RE7, P59400, Q8ABA9, Q5YYQ0, Q3J7H1, Q2YAU5, Q5P790, Q9RH05, Q87C29, Q47QS9, Q5WX91, Q31GY9, P00815, Q3SI67, O59626, Q8CQ95, Q7VQX0, Q5KVC6, P10370, Q8ZY17, Q9PBC5, O33775, Q989E7, Q87WV5, Q5PDP3, P73058, Q845V3, Q6G5Z7, Q465R4, Q3JMZ6, Q4FNE2, Q2P3K3, Q606Q2, Q9HVW9, Q32EE9, Q4JW59, Q8P9P2, Q4A044, P16245, Q3Z878, Q3ZXL7, Q3J079, Q4QN74, Q3BUF7, Q5ZW87, P63951, Q57F99, Q7VA26, Q4FQF8, Q92S26, Q3SW26, P18786, P62458, Q7VFF5, Q8TXG3, Q63Q86, Q62GD9, Q9RQ82, Q8ESR8, Q92E84, Q7N6I1, Q58851, Q8F393, Q2YZB4, Q65RB1, Q5SKC1, Q9HPW5, Q8G2R2, P28736, Q4UU40, Q2RGV8, Q8YSM8, Q7W2Y4, Q8YF59, Q8TL41, Q8R882, Q5HCL9, Q87QL1, Q6FEC8, Q81T62, Q8Y9G1, Q66C49, Q02136, P59398, Q3AD53, Q9CLM4, P62457, Q8KEY6, Q9K6Z2, Q5MZ26, B0SS41, Q9RQ88, Q4ZNV9, Q5HSJ3, Q6ANR3, Q7VSZ1, Q8DGR2, Q97KI2, Q970Y9, Q39K91, Q48EC9, Q47XB8, Q3ICF0, Q81G06, Q2RQM7, Q5E638, Q5WDH8, Q8NNT5, P60858, B0S9F2, P63953, O26327, Q65EF9, Q5HKN8, P60860, Q6GDC6, Q9ZHE6, Q9PM77, Q8EFB1, Q46J19, Q82AA6, Q4J8I8, Q3M5D3, P45353, Q6KZD1, Q9JYH8, Q30TA4, Q57MS3, Q5QWP8, O66976, Q7P0F6, Q39YP7, Q4KI73, P59397, Q5NAY4, O34651, Q6D411, Q9A5V1, Q9RSI4, Q313T7, Q8G4S9, Q9CC57, Q8YWL4, Q8Z5K0, O74712, Q46WL2, Q6HLE7, P62456, Q5V574, P59401, Q9JTH9, Q63DX2, Q8UHX1, Q8ZFX5, Q5JFR5, Q9RQ85, Q5X5W9, Q8D8Q0, P63954, Q9X0D1, Q2YPB8, P24226, P60861, P9WNW8, P44001, P07685, Q7WDY4, P59399, Q7UX39, Q7V5N9, Q8FNZ0, Q82W26, Q8GDP4, Q12670, Q3AR25, Q6AE76, Q6A8L5, P06988, P9WNW9, Q3Z0G5, Q3B5E3, Q3KHZ2, Q8FG52, Q9P777</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -563,31 +563,31 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>15.31924337854084</v>
+        <v>57.98770866620097</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2302083333333333</v>
+        <v>0.8426616915422886</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4604166666666667</v>
+        <v>0.75</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.9353233830845772</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Q8BWN8, Q8VHK0, Q8N9L9, P58137, O14734</t>
+          <t>G2SYC0, B0MC58</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>A1ZAI3, Q8WVX9, B9TSP7, Q0P5J1, Q08891, Q5R834, Q96K12, Q7ZXF5, Q7TNT2, Q5ZM72, Q922J9, Q66H50</t>
+          <t>Q8WVX9, Q5R834, Q7ZXF5, Q5ZM72, Q922J9, Q66H50</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -600,31 +600,31 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>57.98770866620097</v>
+        <v>51.75746525426651</v>
       </c>
       <c r="E5" t="n">
-        <v>0.425</v>
+        <v>0.7026153952459924</v>
       </c>
       <c r="F5" t="n">
-        <v>0.85</v>
+        <v>0.4699074074074074</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.9353233830845772</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>B3EY95</t>
+          <t>Q91VA0, P33124, O06417, Q9QUJ7, P9WQ51, Q63151, O88561, Q2KHW5, Q5R668, Q4R4P9, P18163, Q99PU5, Q7ZYC4, P47912, O88813, P9WQ37, O14975, P97524, O05307, Q8JZR0, O35488, Q91VE0, Q9M0X9, O95573, Q8LPS1, Q5ZKR7, Q9BEA2, Q8LKS5, Q84P21, Q9CZW4, P33121, Q08AH1, Q84P23, P41216, Q5FVE4, Q2XU92, P39518, Q4R3Y4, Q5RDY4, Q91WC3, O53521, O60488, P39002, Q5K4L6, P69451, Q5SKN9, Q9UKU0, Q9ULC5, A1L1K7, O35547, O53551, Q6P1M0, Q924N5, Q96GR2, P30624, Q9JID6</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>A1ZAI3, Q8WVX9, B9TSP7, Q0P5J1, Q08891, Q5R834, Q96K12, Q7ZXF5, Q7TNT2, Q5ZM72, Q922J9, Q66H50</t>
+          <t>Q8WVX9, Q5R834, Q7ZXF5, Q5ZM72, Q922J9, Q66H50</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -637,25 +637,25 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>51.75746525426651</v>
+        <v>15.31924337854084</v>
       </c>
       <c r="E6" t="n">
-        <v>0.276199494949495</v>
+        <v>0.647870024875622</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5523989898989899</v>
+        <v>0.3604166666666667</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.9353233830845772</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>C1DW75, A9A986, Q6G6P8, D1BMT0, C0QSH0, Q6A6M4, A6VHG3, A4FVV0, A6UWX4, C4LK80, D3E0R7, P53559, A6UQM0, D8KN09, Q3A3Z7, P22822, A6QJR2, Q58693, C9REY1, D5VQA3, C9RPK4, Q5HKF3, P67550, B5YK86, Q8NV07, P67549, B2V6W9, A5IVK3, D3G0V0, A7X666, D3SN37, D4H9Y2, Q70JY7, E8VHU4, B8J3V1, A7Z5B6, E0TXE1, Q6LWX9, D3S7P2, Q8CTZ3, Q6NGW9, E3E2E2, O67575, Q2YVY8, D3DK66, E1UV19, A6U4F3, Q2FE74, Q65ML3, Q2FVJ9, Q6GE10, Q5HDD1</t>
+          <t>P0AGG2, P0AGG3</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>A1ZAI3, Q8WVX9, B9TSP7, Q0P5J1, Q08891, Q5R834, Q96K12, Q7ZXF5, Q7TNT2, Q5ZM72, Q922J9, Q66H50</t>
+          <t>Q8WVX9, Q5R834, Q7ZXF5, Q5ZM72, Q922J9, Q66H50</t>
         </is>
       </c>
     </row>

</xml_diff>